<commit_message>
New evaluation of forces using substraction of data points instead of substraction of fit
</commit_message>
<xml_diff>
--- a/force_based/T_vs_F_Wing_Model_Results.xlsx
+++ b/force_based/T_vs_F_Wing_Model_Results.xlsx
@@ -431,7 +431,7 @@
     <t xml:space="preserve">[u.^2,u.^2.*sin(sk).^2,u.^2.*the.*sin(sk).^2,u.^2.*the,u.^2.*the.^2.*sin(sk).^2,u.^2.*the.^2]</t>
   </si>
   <si>
-    <t xml:space="preserve">[-0.008484928911816, 0.001025145266924, 0.153596528756635,-0.005376039316972,0.681068034638300,-0.023838094268066]</t>
+    <t xml:space="preserve">[-0.006428638953316, 0.003532085496834, 0.167195264490172,6.660874387423239e-04,0.594410370645878,0.002368065163524]</t>
   </si>
   <si>
     <t xml:space="preserve">[u.^2.*sin(sk).^2,u.^2,u.^2.*the.*sin(sk).^2,u.^2.*the,u.^2.*the.^2.*sin(sk).^2,u.^2.*the.^2]</t>
@@ -455,10 +455,10 @@
     <t xml:space="preserve">[cos(sk).*u.^2, u.^2, the.*u.^2, theta.^2.*u.^2]</t>
   </si>
   <si>
-    <t xml:space="preserve">[-0.009013405108487   -0.019880356084256     0.000985004818838     0.144397520747447}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.001569295267630     0.005989742907274     -0.234671274859478     0.066122038350159]</t>
+    <t xml:space="preserve">[-0.008111212221499   -0.024771353274546     -0.008297633291171    0.177246306723145}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.004010655576495     -0.000721901291023     -0.112383214091401     0.077819486465484]</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1310,8 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1319,7 +1319,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="86.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.22"/>
@@ -1428,19 +1428,19 @@
         <v>136</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0.389212774803512</v>
+        <v>0.306488942975441</v>
       </c>
       <c r="F5" s="8" t="n">
-        <v>0.020711723833624</v>
+        <v>0.01604872616039</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>1.50331442907306</v>
+        <v>1.51864619175753</v>
       </c>
       <c r="H5" s="8" t="n">
-        <v>0.079997973616826</v>
+        <v>0.079521096681094</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>18.7919063584489</v>
+        <v>19.0974</v>
       </c>
       <c r="J5" s="3" t="n">
         <v>6</v>
@@ -1700,19 +1700,19 @@
         <v>144</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0.240686078575435</v>
+        <v>0.323963710192727</v>
       </c>
       <c r="F17" s="8" t="n">
-        <v>0.034982505099465</v>
+        <v>0.045672975063812</v>
       </c>
       <c r="G17" s="3" t="n">
-        <v>0.741972600057153</v>
+        <v>1.02814195849866</v>
       </c>
       <c r="H17" s="8" t="n">
-        <v>0.132693436450043</v>
+        <v>0.144949266091047</v>
       </c>
       <c r="I17" s="3" t="n">
-        <v>5.5916</v>
+        <v>7.093116</v>
       </c>
       <c r="J17" s="3" t="n">
         <v>4</v>
@@ -1750,19 +1750,19 @@
         <v>145</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.337581651251697</v>
+        <v>0.91801336793276</v>
       </c>
       <c r="F19" s="7" t="n">
-        <v>0.019239806864909</v>
+        <v>0.088860928663791</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>1.00761489914735</v>
+        <v>2.47637296736596</v>
       </c>
       <c r="H19" s="7" t="n">
-        <v>0.057427043152134</v>
+        <v>0.23970544360762</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>17.546</v>
+        <v>10.3309</v>
       </c>
       <c r="J19" s="2" t="n">
         <v>4</v>

</xml_diff>